<commit_message>
Aggiunta colonna Id Materiale mancante
</commit_message>
<xml_diff>
--- a/tables/xls/it/75_Database materiali.xlsx
+++ b/tables/xls/it/75_Database materiali.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>ORGANIZZAZIONE</t>
   </si>
@@ -27,6 +27,9 @@
     <t>CODICE INVENTARIO</t>
   </si>
   <si>
+    <t>ID MATERIALE</t>
+  </si>
+  <si>
     <t>CATEGORIA</t>
   </si>
   <si>
@@ -133,6 +136,9 @@
   </si>
   <si>
     <t>COD. INV.</t>
+  </si>
+  <si>
+    <t>ID MAT.</t>
   </si>
   <si>
     <t>Testo - Elenco di valori</t>
@@ -502,7 +508,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,17 +519,18 @@
     <col min="1" max="1" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="11.711" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="5.856" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="6.998" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="25.851" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="15.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="5.856" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="6.998" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="25.851" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="17.567" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,6 +563,9 @@
       </c>
       <c r="K1" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -570,7 +580,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -578,7 +588,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -612,10 +622,13 @@
       <c r="L1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -627,33 +640,36 @@
         <v>3</v>
       </c>
       <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>6</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>7</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>8</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>9</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>10</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -662,10 +678,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
@@ -680,67 +696,73 @@
         <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="K3" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="L3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>255</v>
@@ -773,270 +795,285 @@
         <v>255</v>
       </c>
       <c r="L6">
+        <v>255</v>
+      </c>
+      <c r="M6">
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="M7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="M9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>38</v>
+      </c>
+      <c r="M10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="M12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>